<commit_message>
regional fuel data loaded
</commit_message>
<xml_diff>
--- a/downloaded_stats/regional_fuel_sales.xlsx
+++ b/downloaded_stats/regional_fuel_sales.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Summer Research\summer-research-2021\downloaded_stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauls\Desktop\Google Drive\Summer Research\summer-research-2021\downloaded_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8F3C754-1645-4DCA-950C-716BC12353BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4E3ABE-2D3F-4EB5-BA69-88FAE13AC854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7425" yWindow="3570" windowWidth="28800" windowHeight="15345" xr2:uid="{F66B81FE-D9A5-43D1-8E50-B4DCBFDE79CC}"/>
+    <workbookView xWindow="7110" yWindow="-19080" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{F66B81FE-D9A5-43D1-8E50-B4DCBFDE79CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Fuel by Regions" sheetId="1" r:id="rId1"/>
     <sheet name="published Fuel Industry" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLMDX" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="64">
   <si>
     <t>SAFC_GEO_Central</t>
   </si>
@@ -250,6 +251,12 @@
   </si>
   <si>
     <t>This Fuel industry level includes any other non-retail and non-fuel, geographic values that are split into a supplementary non-activity region, that is not included in our Anzsic fuel by regions time series on sheet 1.</t>
+  </si>
+  <si>
+    <t>modelled backseries</t>
+  </si>
+  <si>
+    <t>actual</t>
   </si>
 </sst>
 </file>
@@ -717,7 +724,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999E88C4-DA0A-49FC-88F1-AC527E1FC1C8}">
   <dimension ref="A1:BL29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:AD24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3146,6 +3155,10 @@
       <c r="BK24" s="3"/>
       <c r="BL24" s="3"/>
     </row>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="B25" s="3"/>
+      <c r="AA25" s="3"/>
+    </row>
     <row r="26" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>56</v>
@@ -3171,7 +3184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049B92CC-C7B9-4E2B-9868-0B30C143C1B0}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3440,4 +3453,1895 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC6E247-4AB6-43BA-A57B-116207A02CB1}">
+  <dimension ref="A1:T30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="18" width="11.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1909984672.9143493</v>
+      </c>
+      <c r="D2" s="3">
+        <v>70702925.427225992</v>
+      </c>
+      <c r="E2" s="3">
+        <v>618446335.04252529</v>
+      </c>
+      <c r="F2" s="3">
+        <v>208596103.90331867</v>
+      </c>
+      <c r="G2" s="3">
+        <v>119669901.81374848</v>
+      </c>
+      <c r="H2" s="3">
+        <v>15920128.0691645</v>
+      </c>
+      <c r="I2" s="3">
+        <v>60007969.753605008</v>
+      </c>
+      <c r="J2" s="6">
+        <v>48180403.176558003</v>
+      </c>
+      <c r="K2" s="6">
+        <v>109390733.4898726</v>
+      </c>
+      <c r="L2" s="6">
+        <v>163912354.54107267</v>
+      </c>
+      <c r="M2" s="6">
+        <v>22119599.978809796</v>
+      </c>
+      <c r="N2" s="3">
+        <v>273513993.07516026</v>
+      </c>
+      <c r="O2" s="3">
+        <v>98906412.374769002</v>
+      </c>
+      <c r="P2" s="3">
+        <v>40113261.356290586</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>21696183.300180998</v>
+      </c>
+      <c r="R2" s="3">
+        <v>18657596.712669998</v>
+      </c>
+      <c r="S2" s="3">
+        <v>19588517.213747427</v>
+      </c>
+      <c r="T2" s="3">
+        <v>562253.68562999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2053734959.6245873</v>
+      </c>
+      <c r="D3" s="3">
+        <v>76910066.133864492</v>
+      </c>
+      <c r="E3" s="3">
+        <v>684981349.66131222</v>
+      </c>
+      <c r="F3" s="3">
+        <v>218751693.13613236</v>
+      </c>
+      <c r="G3" s="3">
+        <v>130166995.91379479</v>
+      </c>
+      <c r="H3" s="3">
+        <v>17026068.021243799</v>
+      </c>
+      <c r="I3" s="3">
+        <v>61499758.31926249</v>
+      </c>
+      <c r="J3" s="6">
+        <v>50375616.266773008</v>
+      </c>
+      <c r="K3" s="6">
+        <v>109824656.46518351</v>
+      </c>
+      <c r="L3" s="6">
+        <v>173921809.2679683</v>
+      </c>
+      <c r="M3" s="6">
+        <v>24111518.050012298</v>
+      </c>
+      <c r="N3" s="3">
+        <v>294847650.92434508</v>
+      </c>
+      <c r="O3" s="3">
+        <v>104202503.70625699</v>
+      </c>
+      <c r="P3" s="3">
+        <v>44034811.863341093</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>22917281.620937005</v>
+      </c>
+      <c r="R3" s="3">
+        <v>18280979.010439999</v>
+      </c>
+      <c r="S3" s="3">
+        <v>21305277.96145954</v>
+      </c>
+      <c r="T3" s="3">
+        <v>576923.30226000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1891428477.5080812</v>
+      </c>
+      <c r="D4" s="3">
+        <v>70014113.761133</v>
+      </c>
+      <c r="E4" s="3">
+        <v>615241961.50621676</v>
+      </c>
+      <c r="F4" s="3">
+        <v>204195146.69149473</v>
+      </c>
+      <c r="G4" s="3">
+        <v>121752385.83480628</v>
+      </c>
+      <c r="H4" s="3">
+        <v>15620683.2418344</v>
+      </c>
+      <c r="I4" s="3">
+        <v>58439049.220986977</v>
+      </c>
+      <c r="J4" s="6">
+        <v>46712492.709369987</v>
+      </c>
+      <c r="K4" s="6">
+        <v>101807964.99284707</v>
+      </c>
+      <c r="L4" s="6">
+        <v>158067646.36870593</v>
+      </c>
+      <c r="M4" s="6">
+        <v>24636745.754969306</v>
+      </c>
+      <c r="N4" s="3">
+        <v>269525984.61049837</v>
+      </c>
+      <c r="O4" s="3">
+        <v>101484364.83753912</v>
+      </c>
+      <c r="P4" s="3">
+        <v>41275151.769346885</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>25655886.064150997</v>
+      </c>
+      <c r="R4" s="3">
+        <v>15349288.306229999</v>
+      </c>
+      <c r="S4" s="3">
+        <v>21114822.752621002</v>
+      </c>
+      <c r="T4" s="3">
+        <v>534789.08533000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1828728416.4113371</v>
+      </c>
+      <c r="D5" s="3">
+        <v>77436522.145070285</v>
+      </c>
+      <c r="E5" s="3">
+        <v>570282301.56636703</v>
+      </c>
+      <c r="F5" s="3">
+        <v>193322674.65039909</v>
+      </c>
+      <c r="G5" s="3">
+        <v>116744939.70071301</v>
+      </c>
+      <c r="H5" s="3">
+        <v>15042852.917482998</v>
+      </c>
+      <c r="I5" s="3">
+        <v>59998227.393331006</v>
+      </c>
+      <c r="J5" s="6">
+        <v>47769309.604049996</v>
+      </c>
+      <c r="K5" s="6">
+        <v>97462779.502862111</v>
+      </c>
+      <c r="L5" s="6">
+        <v>163937538.97439581</v>
+      </c>
+      <c r="M5" s="6">
+        <v>20510715.812891003</v>
+      </c>
+      <c r="N5" s="3">
+        <v>271620122.17651224</v>
+      </c>
+      <c r="O5" s="3">
+        <v>95133562.546727389</v>
+      </c>
+      <c r="P5" s="3">
+        <v>40039451.942085199</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>22571429.649668001</v>
+      </c>
+      <c r="R5" s="3">
+        <v>16605637.647249999</v>
+      </c>
+      <c r="S5" s="3">
+        <v>19841094.164751999</v>
+      </c>
+      <c r="T5" s="3">
+        <v>409256.01678000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2010212500.0930507</v>
+      </c>
+      <c r="D6" s="3">
+        <v>76861977.638913304</v>
+      </c>
+      <c r="E6" s="3">
+        <v>672964379.22075844</v>
+      </c>
+      <c r="F6" s="3">
+        <v>212177857.76795116</v>
+      </c>
+      <c r="G6" s="3">
+        <v>129977643.78992598</v>
+      </c>
+      <c r="H6" s="3">
+        <v>16277477.214297099</v>
+      </c>
+      <c r="I6" s="3">
+        <v>63728239.138661996</v>
+      </c>
+      <c r="J6" s="6">
+        <v>49364605.712669998</v>
+      </c>
+      <c r="K6" s="6">
+        <v>116090286.49292731</v>
+      </c>
+      <c r="L6" s="6">
+        <v>173321626.26297006</v>
+      </c>
+      <c r="M6" s="6">
+        <v>20097612.227294002</v>
+      </c>
+      <c r="N6" s="3">
+        <v>279057945.32827342</v>
+      </c>
+      <c r="O6" s="3">
+        <v>100125885.4462146</v>
+      </c>
+      <c r="P6" s="3">
+        <v>41815134.876309894</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>21794572.938933998</v>
+      </c>
+      <c r="R6" s="3">
+        <v>16623563.547200002</v>
+      </c>
+      <c r="S6" s="3">
+        <v>19439374.449089602</v>
+      </c>
+      <c r="T6" s="3">
+        <v>494318.04066</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2004337222.5714364</v>
+      </c>
+      <c r="D7" s="3">
+        <v>83121862.944854483</v>
+      </c>
+      <c r="E7" s="3">
+        <v>656770709.68651187</v>
+      </c>
+      <c r="F7" s="3">
+        <v>214188166.48778617</v>
+      </c>
+      <c r="G7" s="3">
+        <v>135664153.89715701</v>
+      </c>
+      <c r="H7" s="3">
+        <v>17030589.093158197</v>
+      </c>
+      <c r="I7" s="3">
+        <v>62652622.526984014</v>
+      </c>
+      <c r="J7" s="6">
+        <v>50187525.73669</v>
+      </c>
+      <c r="K7" s="6">
+        <v>102516688.49700144</v>
+      </c>
+      <c r="L7" s="6">
+        <v>174429048.48726431</v>
+      </c>
+      <c r="M7" s="6">
+        <v>24798526.970405601</v>
+      </c>
+      <c r="N7" s="3">
+        <v>277328974.39034182</v>
+      </c>
+      <c r="O7" s="3">
+        <v>101475770.82999851</v>
+      </c>
+      <c r="P7" s="3">
+        <v>42020226.997598007</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>24939153.870467</v>
+      </c>
+      <c r="R7" s="3">
+        <v>15369533.7641</v>
+      </c>
+      <c r="S7" s="3">
+        <v>21346066.510597996</v>
+      </c>
+      <c r="T7" s="3">
+        <v>497601.88052000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1883118023.3439164</v>
+      </c>
+      <c r="D8" s="3">
+        <v>81607829.788643599</v>
+      </c>
+      <c r="E8" s="3">
+        <v>599976989.01150453</v>
+      </c>
+      <c r="F8" s="3">
+        <v>205859902.87656829</v>
+      </c>
+      <c r="G8" s="3">
+        <v>125218136.73706509</v>
+      </c>
+      <c r="H8" s="3">
+        <v>16250204.178409001</v>
+      </c>
+      <c r="I8" s="3">
+        <v>58515061.388154998</v>
+      </c>
+      <c r="J8" s="6">
+        <v>48023065.79073</v>
+      </c>
+      <c r="K8" s="6">
+        <v>94506461.484189704</v>
+      </c>
+      <c r="L8" s="6">
+        <v>162361364.79164979</v>
+      </c>
+      <c r="M8" s="6">
+        <v>25582454.022243302</v>
+      </c>
+      <c r="N8" s="3">
+        <v>261168078.02700794</v>
+      </c>
+      <c r="O8" s="3">
+        <v>99073807.334757984</v>
+      </c>
+      <c r="P8" s="3">
+        <v>41324377.539978795</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>26799298.677730005</v>
+      </c>
+      <c r="R8" s="3">
+        <v>14455973.144369999</v>
+      </c>
+      <c r="S8" s="3">
+        <v>21952372.539813001</v>
+      </c>
+      <c r="T8" s="3">
+        <v>442646.0111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1764980582.1808429</v>
+      </c>
+      <c r="D9" s="3">
+        <v>73611880.281709507</v>
+      </c>
+      <c r="E9" s="3">
+        <v>573689564.31408262</v>
+      </c>
+      <c r="F9" s="3">
+        <v>174071957.60928342</v>
+      </c>
+      <c r="G9" s="3">
+        <v>123731510.6773067</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14389008.506630197</v>
+      </c>
+      <c r="I9" s="3">
+        <v>54572335.740823008</v>
+      </c>
+      <c r="J9" s="6">
+        <v>46927691.523599997</v>
+      </c>
+      <c r="K9" s="6">
+        <v>90766580.239064723</v>
+      </c>
+      <c r="L9" s="6">
+        <v>162456168.66425356</v>
+      </c>
+      <c r="M9" s="6">
+        <v>19494548.671136234</v>
+      </c>
+      <c r="N9" s="3">
+        <v>251397319.07765087</v>
+      </c>
+      <c r="O9" s="3">
+        <v>88285305.358123511</v>
+      </c>
+      <c r="P9" s="3">
+        <v>37278085.771214396</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>21901228.504419994</v>
+      </c>
+      <c r="R9" s="3">
+        <v>14871818.324450001</v>
+      </c>
+      <c r="S9" s="3">
+        <v>17221418.349803898</v>
+      </c>
+      <c r="T9" s="3">
+        <v>314160.56728999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1865942724.3726156</v>
+      </c>
+      <c r="D10" s="3">
+        <v>75176265.903365776</v>
+      </c>
+      <c r="E10" s="3">
+        <v>630097134.64232993</v>
+      </c>
+      <c r="F10" s="3">
+        <v>205866917.98008531</v>
+      </c>
+      <c r="G10" s="3">
+        <v>128781702.05697519</v>
+      </c>
+      <c r="H10" s="3">
+        <v>14981171.417709501</v>
+      </c>
+      <c r="I10" s="3">
+        <v>49330494.171172693</v>
+      </c>
+      <c r="J10" s="6">
+        <v>46345757.215839989</v>
+      </c>
+      <c r="K10" s="6">
+        <v>95676724.493587002</v>
+      </c>
+      <c r="L10" s="6">
+        <v>163722608.65259978</v>
+      </c>
+      <c r="M10" s="6">
+        <v>19578895.124915004</v>
+      </c>
+      <c r="N10" s="3">
+        <v>253475527.17075473</v>
+      </c>
+      <c r="O10" s="3">
+        <v>91405820.177150905</v>
+      </c>
+      <c r="P10" s="3">
+        <v>37002854.603914008</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>21219187.279489998</v>
+      </c>
+      <c r="R10" s="3">
+        <v>13876724.506820001</v>
+      </c>
+      <c r="S10" s="3">
+        <v>18947730.477385402</v>
+      </c>
+      <c r="T10" s="3">
+        <v>457208.49852000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1995887087.9326313</v>
+      </c>
+      <c r="D11" s="3">
+        <v>84955625.280257896</v>
+      </c>
+      <c r="E11" s="3">
+        <v>669052811.04635906</v>
+      </c>
+      <c r="F11" s="3">
+        <v>218430851.19699427</v>
+      </c>
+      <c r="G11" s="3">
+        <v>135573758.09262046</v>
+      </c>
+      <c r="H11" s="3">
+        <v>16064924.624930801</v>
+      </c>
+      <c r="I11" s="3">
+        <v>59540094.604057007</v>
+      </c>
+      <c r="J11" s="6">
+        <v>48590085.03932</v>
+      </c>
+      <c r="K11" s="6">
+        <v>99569137.095834509</v>
+      </c>
+      <c r="L11" s="6">
+        <v>179353639.71968916</v>
+      </c>
+      <c r="M11" s="6">
+        <v>23273651.500247397</v>
+      </c>
+      <c r="N11" s="3">
+        <v>260112377.32157165</v>
+      </c>
+      <c r="O11" s="3">
+        <v>97843470.818038702</v>
+      </c>
+      <c r="P11" s="3">
+        <v>40769509.713421293</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>24277777.109789997</v>
+      </c>
+      <c r="R11" s="3">
+        <v>16673660.283</v>
+      </c>
+      <c r="S11" s="3">
+        <v>21317856.053439002</v>
+      </c>
+      <c r="T11" s="3">
+        <v>487858.43306000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2049357094.1874528</v>
+      </c>
+      <c r="D12" s="3">
+        <v>87918632.996885791</v>
+      </c>
+      <c r="E12" s="3">
+        <v>659509877.95554626</v>
+      </c>
+      <c r="F12" s="3">
+        <v>223241032.97528279</v>
+      </c>
+      <c r="G12" s="3">
+        <v>140058817.910458</v>
+      </c>
+      <c r="H12" s="3">
+        <v>21272865.451765902</v>
+      </c>
+      <c r="I12" s="3">
+        <v>63790992.178650998</v>
+      </c>
+      <c r="J12" s="6">
+        <v>46780544.236476906</v>
+      </c>
+      <c r="K12" s="6">
+        <v>105915772.34005837</v>
+      </c>
+      <c r="L12" s="6">
+        <v>179329874.42386934</v>
+      </c>
+      <c r="M12" s="6">
+        <v>30565028.199812002</v>
+      </c>
+      <c r="N12" s="3">
+        <v>268302425.26249498</v>
+      </c>
+      <c r="O12" s="3">
+        <v>108524934.84292801</v>
+      </c>
+      <c r="P12" s="3">
+        <v>43827185.255672999</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>30382144.43761</v>
+      </c>
+      <c r="R12" s="3">
+        <v>16318769.510614</v>
+      </c>
+      <c r="S12" s="3">
+        <v>23127694.117816105</v>
+      </c>
+      <c r="T12" s="3">
+        <v>490502.09151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1917201009.7674639</v>
+      </c>
+      <c r="D13" s="3">
+        <v>84287613.780689269</v>
+      </c>
+      <c r="E13" s="3">
+        <v>641820920.08487403</v>
+      </c>
+      <c r="F13" s="3">
+        <v>203925672.63829786</v>
+      </c>
+      <c r="G13" s="3">
+        <v>134131364.47842626</v>
+      </c>
+      <c r="H13" s="3">
+        <v>11092552.274172999</v>
+      </c>
+      <c r="I13" s="3">
+        <v>61902775.828453995</v>
+      </c>
+      <c r="J13" s="6">
+        <v>44705407.049471997</v>
+      </c>
+      <c r="K13" s="6">
+        <v>100538481.9047478</v>
+      </c>
+      <c r="L13" s="6">
+        <v>170479314.40613529</v>
+      </c>
+      <c r="M13" s="6">
+        <v>23625713.186115991</v>
+      </c>
+      <c r="N13" s="3">
+        <v>249607562.81293461</v>
+      </c>
+      <c r="O13" s="3">
+        <v>93497236.816040978</v>
+      </c>
+      <c r="P13" s="3">
+        <v>37232816.184974097</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>25162583.936639994</v>
+      </c>
+      <c r="R13" s="3">
+        <v>15812906.303990001</v>
+      </c>
+      <c r="S13" s="3">
+        <v>19026158.273259003</v>
+      </c>
+      <c r="T13" s="3">
+        <v>351929.80823999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1868805894.2002838</v>
+      </c>
+      <c r="D14" s="3">
+        <v>78362831.210710704</v>
+      </c>
+      <c r="E14" s="3">
+        <v>630391738.34321523</v>
+      </c>
+      <c r="F14" s="3">
+        <v>193150496.12493971</v>
+      </c>
+      <c r="G14" s="3">
+        <v>129674697.71026829</v>
+      </c>
+      <c r="H14" s="3">
+        <v>15905890.533074001</v>
+      </c>
+      <c r="I14" s="3">
+        <v>62177465.403337292</v>
+      </c>
+      <c r="J14" s="6">
+        <v>44275134.182666495</v>
+      </c>
+      <c r="K14" s="6">
+        <v>103789051.54082775</v>
+      </c>
+      <c r="L14" s="6">
+        <v>150387689.49501204</v>
+      </c>
+      <c r="M14" s="6">
+        <v>21339150.936870001</v>
+      </c>
+      <c r="N14" s="3">
+        <v>252057328.99201465</v>
+      </c>
+      <c r="O14" s="3">
+        <v>93215757.117517009</v>
+      </c>
+      <c r="P14" s="3">
+        <v>36157947.701275699</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>23098195.01952</v>
+      </c>
+      <c r="R14" s="3">
+        <v>15138554.89136</v>
+      </c>
+      <c r="S14" s="3">
+        <v>19343501.548074998</v>
+      </c>
+      <c r="T14" s="3">
+        <v>340463.44959999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2120088237.059453</v>
+      </c>
+      <c r="D15" s="3">
+        <v>90020822.645604998</v>
+      </c>
+      <c r="E15" s="3">
+        <v>695892871.90929604</v>
+      </c>
+      <c r="F15" s="3">
+        <v>220634492.44471428</v>
+      </c>
+      <c r="G15" s="3">
+        <v>147203658.6946508</v>
+      </c>
+      <c r="H15" s="3">
+        <v>18450165.0511664</v>
+      </c>
+      <c r="I15" s="3">
+        <v>68122733.126131698</v>
+      </c>
+      <c r="J15" s="6">
+        <v>46652996.481075004</v>
+      </c>
+      <c r="K15" s="6">
+        <v>112607152.03546362</v>
+      </c>
+      <c r="L15" s="6">
+        <v>192827536.30541602</v>
+      </c>
+      <c r="M15" s="6">
+        <v>28003629.299763896</v>
+      </c>
+      <c r="N15" s="3">
+        <v>285781988.22428477</v>
+      </c>
+      <c r="O15" s="3">
+        <v>102665708.6920739</v>
+      </c>
+      <c r="P15" s="3">
+        <v>41635200.385851495</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>28706980.342939999</v>
+      </c>
+      <c r="R15" s="3">
+        <v>18183393.250439998</v>
+      </c>
+      <c r="S15" s="3">
+        <v>22216775.588570002</v>
+      </c>
+      <c r="T15" s="3">
+        <v>482132.58201000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2062184654.831213</v>
+      </c>
+      <c r="D16" s="3">
+        <v>90593767.510909304</v>
+      </c>
+      <c r="E16" s="3">
+        <v>681991393.0196687</v>
+      </c>
+      <c r="F16" s="3">
+        <v>226919427.31895971</v>
+      </c>
+      <c r="G16" s="3">
+        <v>146798063.19210798</v>
+      </c>
+      <c r="H16" s="3">
+        <v>16902628.758557998</v>
+      </c>
+      <c r="I16" s="3">
+        <v>70117790.474319994</v>
+      </c>
+      <c r="J16" s="6">
+        <v>45134728.075802006</v>
+      </c>
+      <c r="K16" s="6">
+        <v>112992333.41935292</v>
+      </c>
+      <c r="L16" s="6">
+        <v>165797124.38343495</v>
+      </c>
+      <c r="M16" s="6">
+        <v>27417149.198779002</v>
+      </c>
+      <c r="N16" s="3">
+        <v>274364298.93074602</v>
+      </c>
+      <c r="O16" s="3">
+        <v>94694491.822219506</v>
+      </c>
+      <c r="P16" s="3">
+        <v>39105841.748979896</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>29449266.615625001</v>
+      </c>
+      <c r="R16" s="3">
+        <v>18170047.09372</v>
+      </c>
+      <c r="S16" s="3">
+        <v>21376840.589340001</v>
+      </c>
+      <c r="T16" s="3">
+        <v>359462.67868999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2051134307.2031906</v>
+      </c>
+      <c r="D17" s="3">
+        <v>90281684.830309838</v>
+      </c>
+      <c r="E17" s="3">
+        <v>703872405.8940053</v>
+      </c>
+      <c r="F17" s="3">
+        <v>215953200.68293431</v>
+      </c>
+      <c r="G17" s="3">
+        <v>147342376.883856</v>
+      </c>
+      <c r="H17" s="3">
+        <v>16100680.342827197</v>
+      </c>
+      <c r="I17" s="3">
+        <v>67891489.495288596</v>
+      </c>
+      <c r="J17" s="6">
+        <v>45024768.922120392</v>
+      </c>
+      <c r="K17" s="6">
+        <v>111283748.52388163</v>
+      </c>
+      <c r="L17" s="6">
+        <v>170697438.30214098</v>
+      </c>
+      <c r="M17" s="6">
+        <v>21627742.0663862</v>
+      </c>
+      <c r="N17" s="3">
+        <v>266899754.16960523</v>
+      </c>
+      <c r="O17" s="3">
+        <v>90339588.98536101</v>
+      </c>
+      <c r="P17" s="3">
+        <v>36596984.779750109</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>30930831.702029999</v>
+      </c>
+      <c r="R17" s="3">
+        <v>16949939.311659999</v>
+      </c>
+      <c r="S17" s="3">
+        <v>18924444.700444002</v>
+      </c>
+      <c r="T17" s="3">
+        <v>417227.61059</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2210379555.5018539</v>
+      </c>
+      <c r="D18" s="3">
+        <v>92990957.853081346</v>
+      </c>
+      <c r="E18" s="3">
+        <v>744443667.21471822</v>
+      </c>
+      <c r="F18" s="3">
+        <v>293483870.06885475</v>
+      </c>
+      <c r="G18" s="3">
+        <v>146875315.27071112</v>
+      </c>
+      <c r="H18" s="3">
+        <v>15768635.1936776</v>
+      </c>
+      <c r="I18" s="3">
+        <v>69713576.263132393</v>
+      </c>
+      <c r="J18" s="6">
+        <v>45811930.211636409</v>
+      </c>
+      <c r="K18" s="6">
+        <v>120082115.09149264</v>
+      </c>
+      <c r="L18" s="6">
+        <v>180196398.611498</v>
+      </c>
+      <c r="M18" s="6">
+        <v>21323249.044333998</v>
+      </c>
+      <c r="N18" s="3">
+        <v>267525775.14971927</v>
+      </c>
+      <c r="O18" s="3">
+        <v>96935758.831725314</v>
+      </c>
+      <c r="P18" s="3">
+        <v>40190972.175310999</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>38757866.61778231</v>
+      </c>
+      <c r="R18" s="3">
+        <v>17423182.041310001</v>
+      </c>
+      <c r="S18" s="3">
+        <v>18380256.79256</v>
+      </c>
+      <c r="T18" s="3">
+        <v>476029.07030999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2364435292.7781134</v>
+      </c>
+      <c r="D19" s="3">
+        <v>103804675.73754078</v>
+      </c>
+      <c r="E19" s="3">
+        <v>793495443.48495913</v>
+      </c>
+      <c r="F19" s="3">
+        <v>332107149.63019747</v>
+      </c>
+      <c r="G19" s="3">
+        <v>159539222.00911337</v>
+      </c>
+      <c r="H19" s="3">
+        <v>16465766.906709997</v>
+      </c>
+      <c r="I19" s="3">
+        <v>72511646.561937988</v>
+      </c>
+      <c r="J19" s="6">
+        <v>37749010.947946593</v>
+      </c>
+      <c r="K19" s="6">
+        <v>115236831.35895276</v>
+      </c>
+      <c r="L19" s="6">
+        <v>202952731.33126003</v>
+      </c>
+      <c r="M19" s="6">
+        <v>26514983.631758999</v>
+      </c>
+      <c r="N19" s="3">
+        <v>274166053.84207588</v>
+      </c>
+      <c r="O19" s="3">
+        <v>101210555.36914386</v>
+      </c>
+      <c r="P19" s="3">
+        <v>43209939.576746106</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>45648857.737650007</v>
+      </c>
+      <c r="R19" s="3">
+        <v>19339679.007260002</v>
+      </c>
+      <c r="S19" s="3">
+        <v>19917511.1195</v>
+      </c>
+      <c r="T19" s="3">
+        <v>565234.52535999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2158121618.2642031</v>
+      </c>
+      <c r="D20" s="3">
+        <v>94076401.465657979</v>
+      </c>
+      <c r="E20" s="3">
+        <v>709835177.8309983</v>
+      </c>
+      <c r="F20" s="3">
+        <v>286988609.20171124</v>
+      </c>
+      <c r="G20" s="3">
+        <v>147748473.230151</v>
+      </c>
+      <c r="H20" s="3">
+        <v>16791624.470849</v>
+      </c>
+      <c r="I20" s="3">
+        <v>67454364.464909002</v>
+      </c>
+      <c r="J20" s="6">
+        <v>42939586.417457707</v>
+      </c>
+      <c r="K20" s="6">
+        <v>114050530.71451375</v>
+      </c>
+      <c r="L20" s="6">
+        <v>190182038.93999404</v>
+      </c>
+      <c r="M20" s="6">
+        <v>26423592.075907994</v>
+      </c>
+      <c r="N20" s="3">
+        <v>243250725.62311608</v>
+      </c>
+      <c r="O20" s="3">
+        <v>98256771.683509856</v>
+      </c>
+      <c r="P20" s="3">
+        <v>40547688.911067218</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>43860926.614150003</v>
+      </c>
+      <c r="R20" s="3">
+        <v>15556095.190230001</v>
+      </c>
+      <c r="S20" s="3">
+        <v>19714547.811349999</v>
+      </c>
+      <c r="T20" s="3">
+        <v>444463.61862999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2165956921.6391034</v>
+      </c>
+      <c r="D21" s="3">
+        <v>91604511.142268836</v>
+      </c>
+      <c r="E21" s="3">
+        <v>729603378.43641615</v>
+      </c>
+      <c r="F21" s="3">
+        <v>284955766.00792676</v>
+      </c>
+      <c r="G21" s="3">
+        <v>148669095.90507197</v>
+      </c>
+      <c r="H21" s="3">
+        <v>16913849.346944001</v>
+      </c>
+      <c r="I21" s="3">
+        <v>65770915.324599005</v>
+      </c>
+      <c r="J21" s="6">
+        <v>47642112.749336503</v>
+      </c>
+      <c r="K21" s="6">
+        <v>113540597.93174504</v>
+      </c>
+      <c r="L21" s="6">
+        <v>191595193.76495004</v>
+      </c>
+      <c r="M21" s="6">
+        <v>22030949.112865902</v>
+      </c>
+      <c r="N21" s="3">
+        <v>240812247.76704833</v>
+      </c>
+      <c r="O21" s="3">
+        <v>100357770.895114</v>
+      </c>
+      <c r="P21" s="3">
+        <v>39837402.062172085</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>41466106.370214872</v>
+      </c>
+      <c r="R21" s="3">
+        <v>13709382.61764</v>
+      </c>
+      <c r="S21" s="3">
+        <v>16953552.360700004</v>
+      </c>
+      <c r="T21" s="3">
+        <v>494089.84409000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2127337449.6628458</v>
+      </c>
+      <c r="D22" s="3">
+        <v>86493611.475430414</v>
+      </c>
+      <c r="E22" s="3">
+        <v>727672223.59597194</v>
+      </c>
+      <c r="F22" s="3">
+        <v>277907256.85064906</v>
+      </c>
+      <c r="G22" s="3">
+        <v>148255419.97334021</v>
+      </c>
+      <c r="H22" s="3">
+        <v>13403943.5909581</v>
+      </c>
+      <c r="I22" s="3">
+        <v>65130596.945197001</v>
+      </c>
+      <c r="J22" s="6">
+        <v>52579706.27156809</v>
+      </c>
+      <c r="K22" s="6">
+        <v>113185005.33867234</v>
+      </c>
+      <c r="L22" s="6">
+        <v>180681661.05283603</v>
+      </c>
+      <c r="M22" s="6">
+        <v>19967152.408735998</v>
+      </c>
+      <c r="N22" s="3">
+        <v>253837370.71352828</v>
+      </c>
+      <c r="O22" s="3">
+        <v>98836258.653702289</v>
+      </c>
+      <c r="P22" s="3">
+        <v>39068938.715079054</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>22628862.939659998</v>
+      </c>
+      <c r="R22" s="3">
+        <v>12011175.736169999</v>
+      </c>
+      <c r="S22" s="3">
+        <v>15318305.424417</v>
+      </c>
+      <c r="T22" s="3">
+        <v>359959.97693</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2320037530.643136</v>
+      </c>
+      <c r="D23" s="3">
+        <v>97750606.121692985</v>
+      </c>
+      <c r="E23" s="3">
+        <v>762677819.87276793</v>
+      </c>
+      <c r="F23" s="3">
+        <v>312301245.28270942</v>
+      </c>
+      <c r="G23" s="3">
+        <v>171918307.56509969</v>
+      </c>
+      <c r="H23" s="3">
+        <v>14549224.522284899</v>
+      </c>
+      <c r="I23" s="3">
+        <v>71982807.338174</v>
+      </c>
+      <c r="J23" s="6">
+        <v>51900206.423586696</v>
+      </c>
+      <c r="K23" s="6">
+        <v>122091667.24380383</v>
+      </c>
+      <c r="L23" s="6">
+        <v>188458161.242625</v>
+      </c>
+      <c r="M23" s="6">
+        <v>26433582.179987002</v>
+      </c>
+      <c r="N23" s="3">
+        <v>278886277.57268721</v>
+      </c>
+      <c r="O23" s="3">
+        <v>114955682.82405181</v>
+      </c>
+      <c r="P23" s="3">
+        <v>47811357.211588696</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>21194025.014139999</v>
+      </c>
+      <c r="R23" s="3">
+        <v>14464098.8285996</v>
+      </c>
+      <c r="S23" s="3">
+        <v>22148952.294098001</v>
+      </c>
+      <c r="T23" s="3">
+        <v>513509.10524</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2206826398.5105114</v>
+      </c>
+      <c r="D24" s="3">
+        <v>94401351.834891558</v>
+      </c>
+      <c r="E24" s="3">
+        <v>693074178.16645503</v>
+      </c>
+      <c r="F24" s="3">
+        <v>312356029.10797006</v>
+      </c>
+      <c r="G24" s="3">
+        <v>163921459.16977915</v>
+      </c>
+      <c r="H24" s="3">
+        <v>15617901.498158043</v>
+      </c>
+      <c r="I24" s="3">
+        <v>68145088.267077997</v>
+      </c>
+      <c r="J24" s="6">
+        <v>46734916.970215008</v>
+      </c>
+      <c r="K24" s="6">
+        <v>117184803.61415528</v>
+      </c>
+      <c r="L24" s="6">
+        <v>181794923.06491405</v>
+      </c>
+      <c r="M24" s="6">
+        <v>26221228.491776798</v>
+      </c>
+      <c r="N24" s="3">
+        <v>269364363.43751246</v>
+      </c>
+      <c r="O24" s="3">
+        <v>107818986.44843259</v>
+      </c>
+      <c r="P24" s="3">
+        <v>43817915.022658408</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>28019958.289549991</v>
+      </c>
+      <c r="R24" s="3">
+        <v>13882730.97923</v>
+      </c>
+      <c r="S24" s="3">
+        <v>24021108.269285001</v>
+      </c>
+      <c r="T24" s="3">
+        <v>449455.87845000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1418918567.2940686</v>
+      </c>
+      <c r="D25" s="3">
+        <v>59131122.382585384</v>
+      </c>
+      <c r="E25" s="3">
+        <v>458050378.19392967</v>
+      </c>
+      <c r="F25" s="3">
+        <v>191449674.26063389</v>
+      </c>
+      <c r="G25" s="3">
+        <v>111710638.185388</v>
+      </c>
+      <c r="H25" s="3">
+        <v>11873971.177014999</v>
+      </c>
+      <c r="I25" s="3">
+        <v>47356678.685326003</v>
+      </c>
+      <c r="J25" s="6">
+        <v>34976520.410907097</v>
+      </c>
+      <c r="K25" s="6">
+        <v>77201084.873740122</v>
+      </c>
+      <c r="L25" s="6">
+        <v>123242518.491256</v>
+      </c>
+      <c r="M25" s="6">
+        <v>13702922.211966202</v>
+      </c>
+      <c r="N25" s="3">
+        <v>165496609.11253607</v>
+      </c>
+      <c r="O25" s="3">
+        <v>59944922.779410981</v>
+      </c>
+      <c r="P25" s="3">
+        <v>27178095.073045999</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>15975858.006459</v>
+      </c>
+      <c r="R25" s="3">
+        <v>7731120.8784259995</v>
+      </c>
+      <c r="S25" s="3">
+        <v>13505189.811493</v>
+      </c>
+      <c r="T25" s="3">
+        <v>391262.75994999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1958945655.1422114</v>
+      </c>
+      <c r="D26" s="3">
+        <v>81631805.196012765</v>
+      </c>
+      <c r="E26" s="3">
+        <v>611208519.0397644</v>
+      </c>
+      <c r="F26" s="3">
+        <v>276418696.49417812</v>
+      </c>
+      <c r="G26" s="3">
+        <v>150129899.10452801</v>
+      </c>
+      <c r="H26" s="3">
+        <v>16274538.886370001</v>
+      </c>
+      <c r="I26" s="3">
+        <v>61243420.496941</v>
+      </c>
+      <c r="J26" s="6">
+        <v>45711598.719281003</v>
+      </c>
+      <c r="K26" s="6">
+        <v>108167499.06878452</v>
+      </c>
+      <c r="L26" s="6">
+        <v>164506868.33362499</v>
+      </c>
+      <c r="M26" s="6">
+        <v>19932507.391113002</v>
+      </c>
+      <c r="N26" s="3">
+        <v>237367586.20255822</v>
+      </c>
+      <c r="O26" s="3">
+        <v>88495306.988958299</v>
+      </c>
+      <c r="P26" s="3">
+        <v>41670949.155585997</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>24288561.843880001</v>
+      </c>
+      <c r="R26" s="3">
+        <v>12019314.21651</v>
+      </c>
+      <c r="S26" s="3">
+        <v>19400792.338891</v>
+      </c>
+      <c r="T26" s="3">
+        <v>477791.66522999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2075619234.3190546</v>
+      </c>
+      <c r="D27" s="3">
+        <v>89194525.863713592</v>
+      </c>
+      <c r="E27" s="3">
+        <v>671851315.84393406</v>
+      </c>
+      <c r="F27" s="3">
+        <v>298853006.53919607</v>
+      </c>
+      <c r="G27" s="3">
+        <v>153160350.64296094</v>
+      </c>
+      <c r="H27" s="3">
+        <v>17261823.593075</v>
+      </c>
+      <c r="I27" s="3">
+        <v>66989880.497279994</v>
+      </c>
+      <c r="J27" s="6">
+        <v>45332250.659238204</v>
+      </c>
+      <c r="K27" s="6">
+        <v>107477069.94837919</v>
+      </c>
+      <c r="L27" s="6">
+        <v>171782176.91595399</v>
+      </c>
+      <c r="M27" s="6">
+        <v>21239068.107793</v>
+      </c>
+      <c r="N27" s="3">
+        <v>242270375.24351066</v>
+      </c>
+      <c r="O27" s="3">
+        <v>90315484.087213993</v>
+      </c>
+      <c r="P27" s="3">
+        <v>40732668.515490003</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>24645796.309329994</v>
+      </c>
+      <c r="R27" s="3">
+        <v>13143119.6919</v>
+      </c>
+      <c r="S27" s="3">
+        <v>21056153.032506</v>
+      </c>
+      <c r="T27" s="3">
+        <v>314168.82757999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2068752488.3071816</v>
+      </c>
+      <c r="D28" s="3">
+        <v>90699868.736985326</v>
+      </c>
+      <c r="E28" s="3">
+        <v>647938283.33285427</v>
+      </c>
+      <c r="F28" s="3">
+        <v>298580280.8370809</v>
+      </c>
+      <c r="G28" s="3">
+        <v>154889767.43689239</v>
+      </c>
+      <c r="H28" s="3">
+        <v>17344389.26498</v>
+      </c>
+      <c r="I28" s="3">
+        <v>68317790.165262997</v>
+      </c>
+      <c r="J28" s="6">
+        <v>44731132.092020296</v>
+      </c>
+      <c r="K28" s="6">
+        <v>110602937.70568343</v>
+      </c>
+      <c r="L28" s="6">
+        <v>166321552.85452706</v>
+      </c>
+      <c r="M28" s="6">
+        <v>22540544.313697997</v>
+      </c>
+      <c r="N28" s="3">
+        <v>241657376.40980411</v>
+      </c>
+      <c r="O28" s="3">
+        <v>101029361.25613198</v>
+      </c>
+      <c r="P28" s="3">
+        <v>40179462.486161903</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>27545465.100729994</v>
+      </c>
+      <c r="R28" s="3">
+        <v>13472845.874989999</v>
+      </c>
+      <c r="S28" s="3">
+        <v>22475027.836339001</v>
+      </c>
+      <c r="T28" s="3">
+        <v>426402.60304000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2153035780.679204</v>
+      </c>
+      <c r="D29" s="3">
+        <v>85944037.917113379</v>
+      </c>
+      <c r="E29" s="3">
+        <v>695487356.75282979</v>
+      </c>
+      <c r="F29" s="3">
+        <v>307965973.74370408</v>
+      </c>
+      <c r="G29" s="3">
+        <v>161782398.58959499</v>
+      </c>
+      <c r="H29" s="3">
+        <v>16978188.161500003</v>
+      </c>
+      <c r="I29" s="3">
+        <v>69936921.768404603</v>
+      </c>
+      <c r="J29" s="6">
+        <v>44382889.690359503</v>
+      </c>
+      <c r="K29" s="6">
+        <v>112012095.35918801</v>
+      </c>
+      <c r="L29" s="6">
+        <v>171898575.92936397</v>
+      </c>
+      <c r="M29" s="6">
+        <v>21801590.943270925</v>
+      </c>
+      <c r="N29" s="3">
+        <v>256121001.02438483</v>
+      </c>
+      <c r="O29" s="3">
+        <v>99956269.874694034</v>
+      </c>
+      <c r="P29" s="3">
+        <v>43804233.18249388</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>27336901.330770001</v>
+      </c>
+      <c r="R29" s="3">
+        <v>13733124.777556999</v>
+      </c>
+      <c r="S29" s="3">
+        <v>23505577.342014998</v>
+      </c>
+      <c r="T29" s="3">
+        <v>388644.29196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1939705947.2599933</v>
+      </c>
+      <c r="D30" s="3">
+        <v>78276982.117490709</v>
+      </c>
+      <c r="E30" s="3">
+        <v>589035906.20922422</v>
+      </c>
+      <c r="F30" s="3">
+        <v>268544497.49559855</v>
+      </c>
+      <c r="G30" s="3">
+        <v>151649122.78311995</v>
+      </c>
+      <c r="H30" s="3">
+        <v>15382030.878967</v>
+      </c>
+      <c r="I30" s="3">
+        <v>65069975.823888004</v>
+      </c>
+      <c r="J30" s="6">
+        <v>42062349.932330012</v>
+      </c>
+      <c r="K30" s="6">
+        <v>100493091.87303399</v>
+      </c>
+      <c r="L30" s="6">
+        <v>159071453.17649734</v>
+      </c>
+      <c r="M30" s="6">
+        <v>20462382.279126409</v>
+      </c>
+      <c r="N30" s="3">
+        <v>250944406.16355214</v>
+      </c>
+      <c r="O30" s="3">
+        <v>91444469.719804004</v>
+      </c>
+      <c r="P30" s="3">
+        <v>44026449.386487</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>26840805.719949998</v>
+      </c>
+      <c r="R30" s="3">
+        <v>13372271.725627</v>
+      </c>
+      <c r="S30" s="3">
+        <v>22529317.017806999</v>
+      </c>
+      <c r="T30" s="3">
+        <v>500434.95749</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>